<commit_message>
UI advances and output modification
</commit_message>
<xml_diff>
--- a/COVID Contagio Argentina v2.0/Input/Input_Politicas.xlsx
+++ b/COVID Contagio Argentina v2.0/Input/Input_Politicas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Desktop\COVID Contagio Argentina 2.0\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\COVID Contagio Argentina v2.0\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED1B58C-DDCB-45C2-A1DE-54F18A0F7747}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1FF64A-77BF-4A60-BB71-B44DB25BE7AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5B0CB94A-B6C2-49A0-86A6-006E3DA04721}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Todas</t>
   </si>
@@ -154,16 +154,10 @@
     <t>08/05/2020</t>
   </si>
   <si>
-    <t>24/05/2020</t>
-  </si>
-  <si>
     <t>24 Partidos del Gran Buenos Aires</t>
   </si>
   <si>
-    <t>20/06/2020</t>
-  </si>
-  <si>
-    <t>04/08/2020</t>
+    <t>13/05/2020</t>
   </si>
 </sst>
 </file>
@@ -858,6 +852,7 @@
       <sheetName val="Agravamiento"/>
       <sheetName val="Tasa de Enfermedad Moderada"/>
       <sheetName val="Tasa de Enfermedad Grave"/>
+      <sheetName val="Input_Simulador"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -879,6 +874,7 @@
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
+      <sheetData sheetId="19" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1236,7 +1232,7 @@
   <dimension ref="A1:K145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,10 +1333,10 @@
         <v>37</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="G3" s="2">
         <v>0.9</v>
@@ -1371,7 +1367,7 @@
         <v>37</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>35</v>
@@ -1391,37 +1387,19 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="A5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UI Changes, added travel impact of policies, got rid of unused code
</commit_message>
<xml_diff>
--- a/COVID Contagio Argentina v2.0/Input/Input_Politicas.xlsx
+++ b/COVID Contagio Argentina v2.0/Input/Input_Politicas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\COVID Contagio Argentina v2.0\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1FF64A-77BF-4A60-BB71-B44DB25BE7AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3D0680-6E66-4C47-A396-E4D86F817BFD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5B0CB94A-B6C2-49A0-86A6-006E3DA04721}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>Todas</t>
   </si>
@@ -121,9 +121,6 @@
     <t>6. Regiones</t>
   </si>
   <si>
-    <t>11. Efecto fronteras</t>
-  </si>
-  <si>
     <t>1. Id</t>
   </si>
   <si>
@@ -158,6 +155,12 @@
   </si>
   <si>
     <t>13/05/2020</t>
+  </si>
+  <si>
+    <t>11. Efecto fronteras internas</t>
+  </si>
+  <si>
+    <t>12. Efecto fronteras externas</t>
   </si>
 </sst>
 </file>
@@ -852,7 +855,6 @@
       <sheetName val="Agravamiento"/>
       <sheetName val="Tasa de Enfermedad Moderada"/>
       <sheetName val="Tasa de Enfermedad Grave"/>
-      <sheetName val="Input_Simulador"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -874,7 +876,6 @@
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
-      <sheetData sheetId="19" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1229,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39070CB-F05F-486C-973E-3F0680FC6C9A}">
-  <dimension ref="A1:K145"/>
+  <dimension ref="A1:L145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,12 +1248,13 @@
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>24</v>
@@ -1261,31 +1263,34 @@
         <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="33" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1296,10 +1301,10 @@
         <v>19</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>0</v>
@@ -1316,9 +1321,14 @@
       <c r="J2" s="2">
         <v>0.5</v>
       </c>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="K2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>+IF(ISBLANK(B3),"",A2+1)</f>
         <v>2</v>
@@ -1330,13 +1340,13 @@
         <v>19</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="G3" s="2">
         <v>0.9</v>
@@ -1350,9 +1360,14 @@
       <c r="J3" s="2">
         <v>0.5</v>
       </c>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" ht="33" x14ac:dyDescent="0.25">
+      <c r="K3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A67" si="0">+IF(ISBLANK(B4),"",A3+1)</f>
         <v>3</v>
@@ -1364,13 +1379,13 @@
         <v>19</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="2">
         <v>0.9</v>
@@ -1384,9 +1399,14 @@
       <c r="J4" s="2">
         <v>0.5</v>
       </c>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1401,8 +1421,9 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1417,8 +1438,9 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1433,8 +1455,9 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1449,8 +1472,9 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1465,8 +1489,9 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1481,8 +1506,9 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1497,8 +1523,9 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1513,8 +1540,9 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1529,8 +1557,9 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1545,8 +1574,9 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1561,8 +1591,9 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1577,8 +1608,9 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1593,8 +1625,9 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1609,8 +1642,9 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1625,8 +1659,9 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1641,8 +1676,9 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1657,8 +1693,9 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1673,8 +1710,9 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1689,8 +1727,9 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1705,8 +1744,9 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1721,8 +1761,9 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1737,8 +1778,9 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1753,8 +1795,9 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1769,8 +1812,9 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1785,8 +1829,9 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1801,8 +1846,9 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1817,8 +1863,9 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1833,8 +1880,9 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1849,8 +1897,9 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1865,8 +1914,9 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1881,8 +1931,9 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1897,8 +1948,9 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1913,8 +1965,9 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1929,8 +1982,9 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1945,8 +1999,9 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-    </row>
-    <row r="40" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1961,8 +2016,9 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1977,8 +2033,9 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1993,8 +2050,9 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2009,8 +2067,9 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-    </row>
-    <row r="44" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2025,8 +2084,9 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-    </row>
-    <row r="45" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2041,8 +2101,9 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-    </row>
-    <row r="46" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2057,8 +2118,9 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2073,8 +2135,9 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-    </row>
-    <row r="48" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2089,8 +2152,9 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-    </row>
-    <row r="49" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2105,8 +2169,9 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-    </row>
-    <row r="50" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2121,8 +2186,9 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-    </row>
-    <row r="51" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2137,8 +2203,9 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
-    </row>
-    <row r="52" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2153,8 +2220,9 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
-    </row>
-    <row r="53" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2169,8 +2237,9 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
-    </row>
-    <row r="54" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2185,8 +2254,9 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
-    </row>
-    <row r="55" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2201,8 +2271,9 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
-    </row>
-    <row r="56" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2217,8 +2288,9 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
-    </row>
-    <row r="57" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2233,8 +2305,9 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
-    </row>
-    <row r="58" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2249,8 +2322,9 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
-    </row>
-    <row r="59" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2265,8 +2339,9 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
-    </row>
-    <row r="60" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2281,8 +2356,9 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
-    </row>
-    <row r="61" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2297,8 +2373,9 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
-    </row>
-    <row r="62" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2313,8 +2390,9 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
-    </row>
-    <row r="63" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2329,8 +2407,9 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
-    </row>
-    <row r="64" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2345,8 +2424,9 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
-    </row>
-    <row r="65" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2361,8 +2441,9 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
-    </row>
-    <row r="66" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2377,8 +2458,9 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
-    </row>
-    <row r="67" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2393,8 +2475,9 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
-    </row>
-    <row r="68" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="str">
         <f t="shared" ref="A68:A131" si="1">+IF(ISBLANK(B68),"",A67+1)</f>
         <v/>
@@ -2409,8 +2492,9 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
-    </row>
-    <row r="69" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2425,8 +2509,9 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
-    </row>
-    <row r="70" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2441,8 +2526,9 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
-    </row>
-    <row r="71" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2457,8 +2543,9 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
-    </row>
-    <row r="72" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L71" s="2"/>
+    </row>
+    <row r="72" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2473,8 +2560,9 @@
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
-    </row>
-    <row r="73" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2489,8 +2577,9 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
-    </row>
-    <row r="74" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L73" s="2"/>
+    </row>
+    <row r="74" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2505,8 +2594,9 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
-    </row>
-    <row r="75" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2521,8 +2611,9 @@
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
-    </row>
-    <row r="76" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L75" s="2"/>
+    </row>
+    <row r="76" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2537,8 +2628,9 @@
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
-    </row>
-    <row r="77" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L76" s="2"/>
+    </row>
+    <row r="77" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2553,8 +2645,9 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
-    </row>
-    <row r="78" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L77" s="2"/>
+    </row>
+    <row r="78" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2569,8 +2662,9 @@
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
-    </row>
-    <row r="79" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L78" s="2"/>
+    </row>
+    <row r="79" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2585,8 +2679,9 @@
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
-    </row>
-    <row r="80" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L79" s="2"/>
+    </row>
+    <row r="80" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2601,8 +2696,9 @@
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
-    </row>
-    <row r="81" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L80" s="2"/>
+    </row>
+    <row r="81" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2617,8 +2713,9 @@
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
-    </row>
-    <row r="82" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L81" s="2"/>
+    </row>
+    <row r="82" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2633,8 +2730,9 @@
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
-    </row>
-    <row r="83" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L82" s="2"/>
+    </row>
+    <row r="83" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2649,8 +2747,9 @@
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
-    </row>
-    <row r="84" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L83" s="2"/>
+    </row>
+    <row r="84" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2665,8 +2764,9 @@
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
-    </row>
-    <row r="85" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L84" s="2"/>
+    </row>
+    <row r="85" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2681,8 +2781,9 @@
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
-    </row>
-    <row r="86" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L85" s="2"/>
+    </row>
+    <row r="86" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2697,8 +2798,9 @@
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
-    </row>
-    <row r="87" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L86" s="2"/>
+    </row>
+    <row r="87" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2713,8 +2815,9 @@
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
-    </row>
-    <row r="88" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L87" s="2"/>
+    </row>
+    <row r="88" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2729,8 +2832,9 @@
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
-    </row>
-    <row r="89" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L88" s="2"/>
+    </row>
+    <row r="89" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2745,8 +2849,9 @@
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
-    </row>
-    <row r="90" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L89" s="2"/>
+    </row>
+    <row r="90" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2761,8 +2866,9 @@
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
-    </row>
-    <row r="91" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L90" s="2"/>
+    </row>
+    <row r="91" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2777,8 +2883,9 @@
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
-    </row>
-    <row r="92" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L91" s="2"/>
+    </row>
+    <row r="92" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2793,8 +2900,9 @@
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
-    </row>
-    <row r="93" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L92" s="2"/>
+    </row>
+    <row r="93" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2809,8 +2917,9 @@
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
-    </row>
-    <row r="94" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L93" s="2"/>
+    </row>
+    <row r="94" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2825,8 +2934,9 @@
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
-    </row>
-    <row r="95" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L94" s="2"/>
+    </row>
+    <row r="95" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2841,8 +2951,9 @@
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
-    </row>
-    <row r="96" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L95" s="2"/>
+    </row>
+    <row r="96" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2857,8 +2968,9 @@
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
-    </row>
-    <row r="97" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L96" s="2"/>
+    </row>
+    <row r="97" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2873,8 +2985,9 @@
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
-    </row>
-    <row r="98" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L97" s="2"/>
+    </row>
+    <row r="98" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2889,8 +3002,9 @@
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
-    </row>
-    <row r="99" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L98" s="2"/>
+    </row>
+    <row r="99" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2905,8 +3019,9 @@
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
-    </row>
-    <row r="100" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L99" s="2"/>
+    </row>
+    <row r="100" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2921,8 +3036,9 @@
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
-    </row>
-    <row r="101" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L100" s="2"/>
+    </row>
+    <row r="101" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2937,8 +3053,9 @@
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
-    </row>
-    <row r="102" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L101" s="2"/>
+    </row>
+    <row r="102" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2953,8 +3070,9 @@
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
-    </row>
-    <row r="103" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L102" s="2"/>
+    </row>
+    <row r="103" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2969,8 +3087,9 @@
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
-    </row>
-    <row r="104" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L103" s="2"/>
+    </row>
+    <row r="104" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2985,8 +3104,9 @@
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
-    </row>
-    <row r="105" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L104" s="2"/>
+    </row>
+    <row r="105" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3001,8 +3121,9 @@
       <c r="I105" s="2"/>
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
-    </row>
-    <row r="106" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L105" s="2"/>
+    </row>
+    <row r="106" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3017,8 +3138,9 @@
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
-    </row>
-    <row r="107" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L106" s="2"/>
+    </row>
+    <row r="107" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3033,8 +3155,9 @@
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
-    </row>
-    <row r="108" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L107" s="2"/>
+    </row>
+    <row r="108" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3049,8 +3172,9 @@
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
-    </row>
-    <row r="109" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L108" s="2"/>
+    </row>
+    <row r="109" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3065,8 +3189,9 @@
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
-    </row>
-    <row r="110" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L109" s="2"/>
+    </row>
+    <row r="110" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3081,8 +3206,9 @@
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
-    </row>
-    <row r="111" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L110" s="2"/>
+    </row>
+    <row r="111" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3097,8 +3223,9 @@
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
-    </row>
-    <row r="112" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L111" s="2"/>
+    </row>
+    <row r="112" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3113,8 +3240,9 @@
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
-    </row>
-    <row r="113" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L112" s="2"/>
+    </row>
+    <row r="113" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3129,8 +3257,9 @@
       <c r="I113" s="2"/>
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
-    </row>
-    <row r="114" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L113" s="2"/>
+    </row>
+    <row r="114" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3145,8 +3274,9 @@
       <c r="I114" s="2"/>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
-    </row>
-    <row r="115" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L114" s="2"/>
+    </row>
+    <row r="115" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3161,8 +3291,9 @@
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
-    </row>
-    <row r="116" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L115" s="2"/>
+    </row>
+    <row r="116" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3177,8 +3308,9 @@
       <c r="I116" s="2"/>
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
-    </row>
-    <row r="117" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L116" s="2"/>
+    </row>
+    <row r="117" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3193,8 +3325,9 @@
       <c r="I117" s="2"/>
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>
-    </row>
-    <row r="118" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L117" s="2"/>
+    </row>
+    <row r="118" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3209,8 +3342,9 @@
       <c r="I118" s="2"/>
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
-    </row>
-    <row r="119" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L118" s="2"/>
+    </row>
+    <row r="119" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3225,8 +3359,9 @@
       <c r="I119" s="2"/>
       <c r="J119" s="2"/>
       <c r="K119" s="2"/>
-    </row>
-    <row r="120" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L119" s="2"/>
+    </row>
+    <row r="120" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3241,8 +3376,9 @@
       <c r="I120" s="2"/>
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
-    </row>
-    <row r="121" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L120" s="2"/>
+    </row>
+    <row r="121" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3257,8 +3393,9 @@
       <c r="I121" s="2"/>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
-    </row>
-    <row r="122" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L121" s="2"/>
+    </row>
+    <row r="122" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3273,8 +3410,9 @@
       <c r="I122" s="2"/>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
-    </row>
-    <row r="123" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L122" s="2"/>
+    </row>
+    <row r="123" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3289,8 +3427,9 @@
       <c r="I123" s="2"/>
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
-    </row>
-    <row r="124" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L123" s="2"/>
+    </row>
+    <row r="124" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3305,8 +3444,9 @@
       <c r="I124" s="2"/>
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
-    </row>
-    <row r="125" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L124" s="2"/>
+    </row>
+    <row r="125" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3321,8 +3461,9 @@
       <c r="I125" s="2"/>
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
-    </row>
-    <row r="126" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L125" s="2"/>
+    </row>
+    <row r="126" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3337,8 +3478,9 @@
       <c r="I126" s="2"/>
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
-    </row>
-    <row r="127" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L126" s="2"/>
+    </row>
+    <row r="127" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3353,8 +3495,9 @@
       <c r="I127" s="2"/>
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
-    </row>
-    <row r="128" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L127" s="2"/>
+    </row>
+    <row r="128" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3369,8 +3512,9 @@
       <c r="I128" s="2"/>
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
-    </row>
-    <row r="129" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L128" s="2"/>
+    </row>
+    <row r="129" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3385,8 +3529,9 @@
       <c r="I129" s="2"/>
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
-    </row>
-    <row r="130" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L129" s="2"/>
+    </row>
+    <row r="130" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3401,8 +3546,9 @@
       <c r="I130" s="2"/>
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
-    </row>
-    <row r="131" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L130" s="2"/>
+    </row>
+    <row r="131" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3417,8 +3563,9 @@
       <c r="I131" s="2"/>
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
-    </row>
-    <row r="132" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L131" s="2"/>
+    </row>
+    <row r="132" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="str">
         <f t="shared" ref="A132:A145" si="2">+IF(ISBLANK(B132),"",A131+1)</f>
         <v/>
@@ -3433,8 +3580,9 @@
       <c r="I132" s="2"/>
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
-    </row>
-    <row r="133" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L132" s="2"/>
+    </row>
+    <row r="133" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3449,8 +3597,9 @@
       <c r="I133" s="2"/>
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
-    </row>
-    <row r="134" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L133" s="2"/>
+    </row>
+    <row r="134" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3465,8 +3614,9 @@
       <c r="I134" s="2"/>
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
-    </row>
-    <row r="135" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L134" s="2"/>
+    </row>
+    <row r="135" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3481,8 +3631,9 @@
       <c r="I135" s="2"/>
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
-    </row>
-    <row r="136" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L135" s="2"/>
+    </row>
+    <row r="136" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3497,8 +3648,9 @@
       <c r="I136" s="2"/>
       <c r="J136" s="2"/>
       <c r="K136" s="2"/>
-    </row>
-    <row r="137" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L136" s="2"/>
+    </row>
+    <row r="137" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3513,8 +3665,9 @@
       <c r="I137" s="2"/>
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
-    </row>
-    <row r="138" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L137" s="2"/>
+    </row>
+    <row r="138" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3529,8 +3682,9 @@
       <c r="I138" s="2"/>
       <c r="J138" s="2"/>
       <c r="K138" s="2"/>
-    </row>
-    <row r="139" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L138" s="2"/>
+    </row>
+    <row r="139" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3545,8 +3699,9 @@
       <c r="I139" s="2"/>
       <c r="J139" s="2"/>
       <c r="K139" s="2"/>
-    </row>
-    <row r="140" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L139" s="2"/>
+    </row>
+    <row r="140" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3561,8 +3716,9 @@
       <c r="I140" s="2"/>
       <c r="J140" s="2"/>
       <c r="K140" s="2"/>
-    </row>
-    <row r="141" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L140" s="2"/>
+    </row>
+    <row r="141" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3577,8 +3733,9 @@
       <c r="I141" s="2"/>
       <c r="J141" s="2"/>
       <c r="K141" s="2"/>
-    </row>
-    <row r="142" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L141" s="2"/>
+    </row>
+    <row r="142" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3593,8 +3750,9 @@
       <c r="I142" s="2"/>
       <c r="J142" s="2"/>
       <c r="K142" s="2"/>
-    </row>
-    <row r="143" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L142" s="2"/>
+    </row>
+    <row r="143" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3609,8 +3767,9 @@
       <c r="I143" s="2"/>
       <c r="J143" s="2"/>
       <c r="K143" s="2"/>
-    </row>
-    <row r="144" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L143" s="2"/>
+    </row>
+    <row r="144" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3625,8 +3784,9 @@
       <c r="I144" s="2"/>
       <c r="J144" s="2"/>
       <c r="K144" s="2"/>
-    </row>
-    <row r="145" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L144" s="2"/>
+    </row>
+    <row r="145" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3641,6 +3801,7 @@
       <c r="I145" s="2"/>
       <c r="J145" s="2"/>
       <c r="K145" s="2"/>
+      <c r="L145" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="27" type="noConversion"/>
@@ -3689,7 +3850,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Runs tests arrival function. Fix several bugs
</commit_message>
<xml_diff>
--- a/COVID Contagio Argentina v2.0/Input/Input_Politicas.xlsx
+++ b/COVID Contagio Argentina v2.0/Input/Input_Politicas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\P R O J E C T O S\COVID 19\COVID-19-Simulation-Argentina\COVID Contagio Argentina v2.0\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patricio.ivan.pipp\Documents\Modelos\COVID Contagion Argentina\COVID Contagio Argentina v2.0\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8364885F-411D-4DCB-B8AF-314DEEE3DC3B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0E0B8D-59AE-490F-B8FB-D1D7569C27E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2715" windowWidth="25875" windowHeight="11505" xr2:uid="{5B0CB94A-B6C2-49A0-86A6-006E3DA04721}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5B0CB94A-B6C2-49A0-86A6-006E3DA04721}"/>
   </bookViews>
   <sheets>
     <sheet name="Políticas Aplicadas" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Todas</t>
   </si>
@@ -740,7 +740,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -902,6 +902,7 @@
       <sheetName val="Agravamiento"/>
       <sheetName val="Tasa de Enfermedad Moderada"/>
       <sheetName val="Tasa de Enfermedad Grave"/>
+      <sheetName val="Input_Simulador"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -923,6 +924,7 @@
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
+      <sheetData sheetId="19" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1279,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39070CB-F05F-486C-973E-3F0680FC6C9A}">
   <dimension ref="A1:L145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3906,15 +3908,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDC1F280-FE1D-4757-B477-BE607AE2110A}">
   <dimension ref="A1:C151"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3924,7 +3924,7 @@
       <c r="B1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3935,7 +3935,7 @@
       <c r="B2" s="7">
         <v>15000</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3947,8 +3947,8 @@
       <c r="B3" s="7">
         <v>500</v>
       </c>
-      <c r="C3" s="12">
-        <v>43835</v>
+      <c r="C3" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
@@ -3957,7 +3957,7 @@
         <v/>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="str">
@@ -3965,7 +3965,7 @@
         <v/>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="str">
@@ -3973,7 +3973,7 @@
         <v/>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="str">
@@ -3981,7 +3981,7 @@
         <v/>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
@@ -3989,7 +3989,7 @@
         <v/>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
@@ -3997,7 +3997,7 @@
         <v/>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
@@ -4005,7 +4005,7 @@
         <v/>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
@@ -4013,7 +4013,7 @@
         <v/>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
@@ -4021,7 +4021,7 @@
         <v/>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -4029,7 +4029,7 @@
         <v/>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
@@ -4037,7 +4037,7 @@
         <v/>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
@@ -4045,7 +4045,7 @@
         <v/>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
@@ -4053,7 +4053,7 @@
         <v/>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
@@ -4061,7 +4061,7 @@
         <v/>
       </c>
       <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
@@ -4069,7 +4069,7 @@
         <v/>
       </c>
       <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
@@ -4077,7 +4077,7 @@
         <v/>
       </c>
       <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
@@ -4085,7 +4085,7 @@
         <v/>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
@@ -4093,7 +4093,7 @@
         <v/>
       </c>
       <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+      <c r="C21" s="9"/>
     </row>
     <row r="22" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -4101,7 +4101,7 @@
         <v/>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
@@ -4109,7 +4109,7 @@
         <v/>
       </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
@@ -4117,7 +4117,7 @@
         <v/>
       </c>
       <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="C24" s="9"/>
     </row>
     <row r="25" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
@@ -4125,7 +4125,7 @@
         <v/>
       </c>
       <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="str">
@@ -4133,7 +4133,7 @@
         <v/>
       </c>
       <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="str">
@@ -4141,7 +4141,7 @@
         <v/>
       </c>
       <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="str">
@@ -4149,7 +4149,7 @@
         <v/>
       </c>
       <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="str">
@@ -4157,7 +4157,7 @@
         <v/>
       </c>
       <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
+      <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="str">
@@ -4165,7 +4165,7 @@
         <v/>
       </c>
       <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -4173,7 +4173,7 @@
         <v/>
       </c>
       <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="C31" s="9"/>
     </row>
     <row r="32" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="str">
@@ -4181,7 +4181,7 @@
         <v/>
       </c>
       <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="str">
@@ -4189,7 +4189,7 @@
         <v/>
       </c>
       <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
+      <c r="C33" s="9"/>
     </row>
     <row r="34" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="str">
@@ -4197,7 +4197,7 @@
         <v/>
       </c>
       <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="str">
@@ -4205,7 +4205,7 @@
         <v/>
       </c>
       <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
+      <c r="C35" s="9"/>
     </row>
     <row r="36" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="str">
@@ -4213,7 +4213,7 @@
         <v/>
       </c>
       <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="str">
@@ -4221,7 +4221,7 @@
         <v/>
       </c>
       <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
+      <c r="C37" s="9"/>
     </row>
     <row r="38" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="str">
@@ -4229,7 +4229,7 @@
         <v/>
       </c>
       <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
+      <c r="C38" s="9"/>
     </row>
     <row r="39" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="str">
@@ -4237,7 +4237,7 @@
         <v/>
       </c>
       <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
+      <c r="C39" s="9"/>
     </row>
     <row r="40" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -4245,7 +4245,7 @@
         <v/>
       </c>
       <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="str">
@@ -4253,7 +4253,7 @@
         <v/>
       </c>
       <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
+      <c r="C41" s="9"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="str">
@@ -4261,7 +4261,7 @@
         <v/>
       </c>
       <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
+      <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="str">
@@ -4269,7 +4269,7 @@
         <v/>
       </c>
       <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
+      <c r="C43" s="9"/>
     </row>
     <row r="44" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="str">
@@ -4277,7 +4277,7 @@
         <v/>
       </c>
       <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
+      <c r="C44" s="9"/>
     </row>
     <row r="45" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="str">
@@ -4285,7 +4285,7 @@
         <v/>
       </c>
       <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
+      <c r="C45" s="9"/>
     </row>
     <row r="46" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="str">
@@ -4293,7 +4293,7 @@
         <v/>
       </c>
       <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
+      <c r="C46" s="9"/>
     </row>
     <row r="47" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="str">
@@ -4301,7 +4301,7 @@
         <v/>
       </c>
       <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
+      <c r="C47" s="9"/>
     </row>
     <row r="48" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="str">
@@ -4309,7 +4309,7 @@
         <v/>
       </c>
       <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
+      <c r="C48" s="9"/>
     </row>
     <row r="49" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -4317,7 +4317,7 @@
         <v/>
       </c>
       <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
+      <c r="C49" s="9"/>
     </row>
     <row r="50" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="str">
@@ -4325,7 +4325,7 @@
         <v/>
       </c>
       <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
+      <c r="C50" s="9"/>
     </row>
     <row r="51" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="str">
@@ -4333,7 +4333,7 @@
         <v/>
       </c>
       <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
+      <c r="C51" s="9"/>
     </row>
     <row r="52" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="str">
@@ -4341,7 +4341,7 @@
         <v/>
       </c>
       <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
+      <c r="C52" s="9"/>
     </row>
     <row r="53" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="str">
@@ -4349,7 +4349,7 @@
         <v/>
       </c>
       <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
+      <c r="C53" s="9"/>
     </row>
     <row r="54" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="str">
@@ -4357,7 +4357,7 @@
         <v/>
       </c>
       <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
+      <c r="C54" s="9"/>
     </row>
     <row r="55" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="str">
@@ -4365,7 +4365,7 @@
         <v/>
       </c>
       <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
+      <c r="C55" s="9"/>
     </row>
     <row r="56" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="str">
@@ -4373,7 +4373,7 @@
         <v/>
       </c>
       <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
+      <c r="C56" s="9"/>
     </row>
     <row r="57" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="str">
@@ -4381,7 +4381,7 @@
         <v/>
       </c>
       <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
+      <c r="C57" s="9"/>
     </row>
     <row r="58" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -4389,7 +4389,7 @@
         <v/>
       </c>
       <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
+      <c r="C58" s="9"/>
     </row>
     <row r="59" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="str">
@@ -4397,7 +4397,7 @@
         <v/>
       </c>
       <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
+      <c r="C59" s="9"/>
     </row>
     <row r="60" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="str">
@@ -4405,7 +4405,7 @@
         <v/>
       </c>
       <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
+      <c r="C60" s="9"/>
     </row>
     <row r="61" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="str">
@@ -4413,7 +4413,7 @@
         <v/>
       </c>
       <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
+      <c r="C61" s="9"/>
     </row>
     <row r="62" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="str">
@@ -4421,7 +4421,7 @@
         <v/>
       </c>
       <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
+      <c r="C62" s="9"/>
     </row>
     <row r="63" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="str">
@@ -4429,7 +4429,7 @@
         <v/>
       </c>
       <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
+      <c r="C63" s="9"/>
     </row>
     <row r="64" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="str">
@@ -4437,7 +4437,7 @@
         <v/>
       </c>
       <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
+      <c r="C64" s="9"/>
     </row>
     <row r="65" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="str">
@@ -4445,7 +4445,7 @@
         <v/>
       </c>
       <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
+      <c r="C65" s="9"/>
     </row>
     <row r="66" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="str">
@@ -4453,7 +4453,7 @@
         <v/>
       </c>
       <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
+      <c r="C66" s="9"/>
     </row>
     <row r="67" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -4461,7 +4461,7 @@
         <v/>
       </c>
       <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
+      <c r="C67" s="9"/>
     </row>
     <row r="68" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="str">
@@ -4469,7 +4469,7 @@
         <v/>
       </c>
       <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
+      <c r="C68" s="9"/>
     </row>
     <row r="69" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="str">
@@ -4477,7 +4477,7 @@
         <v/>
       </c>
       <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
+      <c r="C69" s="9"/>
     </row>
     <row r="70" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="str">
@@ -4485,7 +4485,7 @@
         <v/>
       </c>
       <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
+      <c r="C70" s="9"/>
     </row>
     <row r="71" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="str">
@@ -4493,7 +4493,7 @@
         <v/>
       </c>
       <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
+      <c r="C71" s="9"/>
     </row>
     <row r="72" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="str">
@@ -4501,7 +4501,7 @@
         <v/>
       </c>
       <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
+      <c r="C72" s="9"/>
     </row>
     <row r="73" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="str">
@@ -4509,7 +4509,7 @@
         <v/>
       </c>
       <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
+      <c r="C73" s="9"/>
     </row>
     <row r="74" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="str">
@@ -4517,7 +4517,7 @@
         <v/>
       </c>
       <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
+      <c r="C74" s="9"/>
     </row>
     <row r="75" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="str">
@@ -4525,7 +4525,7 @@
         <v/>
       </c>
       <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
+      <c r="C75" s="9"/>
     </row>
     <row r="76" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -4533,7 +4533,7 @@
         <v/>
       </c>
       <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
+      <c r="C76" s="9"/>
     </row>
     <row r="77" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="str">
@@ -4541,7 +4541,7 @@
         <v/>
       </c>
       <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
+      <c r="C77" s="9"/>
     </row>
     <row r="78" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="str">
@@ -4549,7 +4549,7 @@
         <v/>
       </c>
       <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
+      <c r="C78" s="9"/>
     </row>
     <row r="79" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="str">
@@ -4557,7 +4557,7 @@
         <v/>
       </c>
       <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
+      <c r="C79" s="9"/>
     </row>
     <row r="80" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="str">
@@ -4565,7 +4565,7 @@
         <v/>
       </c>
       <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
+      <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="str">
@@ -4573,7 +4573,7 @@
         <v/>
       </c>
       <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
+      <c r="C81" s="9"/>
     </row>
     <row r="82" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="str">
@@ -4581,7 +4581,7 @@
         <v/>
       </c>
       <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
+      <c r="C82" s="9"/>
     </row>
     <row r="83" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="str">
@@ -4589,7 +4589,7 @@
         <v/>
       </c>
       <c r="B83" s="7"/>
-      <c r="C83" s="7"/>
+      <c r="C83" s="9"/>
     </row>
     <row r="84" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="str">
@@ -4597,7 +4597,7 @@
         <v/>
       </c>
       <c r="B84" s="7"/>
-      <c r="C84" s="7"/>
+      <c r="C84" s="9"/>
     </row>
     <row r="85" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -4605,7 +4605,7 @@
         <v/>
       </c>
       <c r="B85" s="7"/>
-      <c r="C85" s="7"/>
+      <c r="C85" s="9"/>
     </row>
     <row r="86" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="str">
@@ -4613,7 +4613,7 @@
         <v/>
       </c>
       <c r="B86" s="7"/>
-      <c r="C86" s="7"/>
+      <c r="C86" s="9"/>
     </row>
     <row r="87" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="str">
@@ -4621,7 +4621,7 @@
         <v/>
       </c>
       <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
+      <c r="C87" s="9"/>
     </row>
     <row r="88" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="str">
@@ -4629,7 +4629,7 @@
         <v/>
       </c>
       <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
+      <c r="C88" s="9"/>
     </row>
     <row r="89" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="str">
@@ -4637,7 +4637,7 @@
         <v/>
       </c>
       <c r="B89" s="7"/>
-      <c r="C89" s="7"/>
+      <c r="C89" s="9"/>
     </row>
     <row r="90" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="str">
@@ -4645,7 +4645,7 @@
         <v/>
       </c>
       <c r="B90" s="7"/>
-      <c r="C90" s="7"/>
+      <c r="C90" s="9"/>
     </row>
     <row r="91" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="str">
@@ -4653,7 +4653,7 @@
         <v/>
       </c>
       <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
+      <c r="C91" s="9"/>
     </row>
     <row r="92" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="str">
@@ -4661,7 +4661,7 @@
         <v/>
       </c>
       <c r="B92" s="7"/>
-      <c r="C92" s="7"/>
+      <c r="C92" s="9"/>
     </row>
     <row r="93" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="str">
@@ -4669,7 +4669,7 @@
         <v/>
       </c>
       <c r="B93" s="7"/>
-      <c r="C93" s="7"/>
+      <c r="C93" s="9"/>
     </row>
     <row r="94" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="str">
@@ -4677,7 +4677,7 @@
         <v/>
       </c>
       <c r="B94" s="7"/>
-      <c r="C94" s="7"/>
+      <c r="C94" s="9"/>
     </row>
     <row r="95" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="str">
@@ -4685,7 +4685,7 @@
         <v/>
       </c>
       <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
+      <c r="C95" s="9"/>
     </row>
     <row r="96" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="str">
@@ -4693,7 +4693,7 @@
         <v/>
       </c>
       <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
+      <c r="C96" s="9"/>
     </row>
     <row r="97" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="str">
@@ -4701,7 +4701,7 @@
         <v/>
       </c>
       <c r="B97" s="7"/>
-      <c r="C97" s="7"/>
+      <c r="C97" s="9"/>
     </row>
     <row r="98" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="str">
@@ -4709,7 +4709,7 @@
         <v/>
       </c>
       <c r="B98" s="7"/>
-      <c r="C98" s="7"/>
+      <c r="C98" s="9"/>
     </row>
     <row r="99" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="str">
@@ -4717,7 +4717,7 @@
         <v/>
       </c>
       <c r="B99" s="7"/>
-      <c r="C99" s="7"/>
+      <c r="C99" s="9"/>
     </row>
     <row r="100" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="str">
@@ -4725,7 +4725,7 @@
         <v/>
       </c>
       <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
+      <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="str">
@@ -4733,7 +4733,7 @@
         <v/>
       </c>
       <c r="B101" s="7"/>
-      <c r="C101" s="7"/>
+      <c r="C101" s="9"/>
     </row>
     <row r="102" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="str">
@@ -4741,7 +4741,7 @@
         <v/>
       </c>
       <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
+      <c r="C102" s="9"/>
     </row>
     <row r="103" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="str">
@@ -4749,7 +4749,7 @@
         <v/>
       </c>
       <c r="B103" s="7"/>
-      <c r="C103" s="7"/>
+      <c r="C103" s="9"/>
     </row>
     <row r="104" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="str">
@@ -4757,7 +4757,7 @@
         <v/>
       </c>
       <c r="B104" s="7"/>
-      <c r="C104" s="7"/>
+      <c r="C104" s="9"/>
     </row>
     <row r="105" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="str">
@@ -4765,7 +4765,7 @@
         <v/>
       </c>
       <c r="B105" s="7"/>
-      <c r="C105" s="7"/>
+      <c r="C105" s="9"/>
     </row>
     <row r="106" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="str">
@@ -4773,7 +4773,7 @@
         <v/>
       </c>
       <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
+      <c r="C106" s="9"/>
     </row>
     <row r="107" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="str">
@@ -4781,7 +4781,7 @@
         <v/>
       </c>
       <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
+      <c r="C107" s="9"/>
     </row>
     <row r="108" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="str">
@@ -4789,7 +4789,7 @@
         <v/>
       </c>
       <c r="B108" s="7"/>
-      <c r="C108" s="7"/>
+      <c r="C108" s="9"/>
     </row>
     <row r="109" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="str">
@@ -4797,7 +4797,7 @@
         <v/>
       </c>
       <c r="B109" s="7"/>
-      <c r="C109" s="7"/>
+      <c r="C109" s="9"/>
     </row>
     <row r="110" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="str">
@@ -4805,7 +4805,7 @@
         <v/>
       </c>
       <c r="B110" s="7"/>
-      <c r="C110" s="7"/>
+      <c r="C110" s="9"/>
     </row>
     <row r="111" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="str">
@@ -4813,7 +4813,7 @@
         <v/>
       </c>
       <c r="B111" s="7"/>
-      <c r="C111" s="7"/>
+      <c r="C111" s="9"/>
     </row>
     <row r="112" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="str">
@@ -4821,7 +4821,7 @@
         <v/>
       </c>
       <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
+      <c r="C112" s="9"/>
     </row>
     <row r="113" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="str">
@@ -4829,7 +4829,7 @@
         <v/>
       </c>
       <c r="B113" s="7"/>
-      <c r="C113" s="7"/>
+      <c r="C113" s="9"/>
     </row>
     <row r="114" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="str">
@@ -4837,7 +4837,7 @@
         <v/>
       </c>
       <c r="B114" s="7"/>
-      <c r="C114" s="7"/>
+      <c r="C114" s="9"/>
     </row>
     <row r="115" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="str">
@@ -4845,7 +4845,7 @@
         <v/>
       </c>
       <c r="B115" s="7"/>
-      <c r="C115" s="7"/>
+      <c r="C115" s="9"/>
     </row>
     <row r="116" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="str">
@@ -4853,7 +4853,7 @@
         <v/>
       </c>
       <c r="B116" s="7"/>
-      <c r="C116" s="7"/>
+      <c r="C116" s="9"/>
     </row>
     <row r="117" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="str">
@@ -4861,7 +4861,7 @@
         <v/>
       </c>
       <c r="B117" s="7"/>
-      <c r="C117" s="7"/>
+      <c r="C117" s="9"/>
     </row>
     <row r="118" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="str">
@@ -4869,7 +4869,7 @@
         <v/>
       </c>
       <c r="B118" s="7"/>
-      <c r="C118" s="7"/>
+      <c r="C118" s="9"/>
     </row>
     <row r="119" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="str">
@@ -4877,7 +4877,7 @@
         <v/>
       </c>
       <c r="B119" s="7"/>
-      <c r="C119" s="7"/>
+      <c r="C119" s="9"/>
     </row>
     <row r="120" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="str">
@@ -4885,7 +4885,7 @@
         <v/>
       </c>
       <c r="B120" s="7"/>
-      <c r="C120" s="7"/>
+      <c r="C120" s="9"/>
     </row>
     <row r="121" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="str">
@@ -4893,7 +4893,7 @@
         <v/>
       </c>
       <c r="B121" s="7"/>
-      <c r="C121" s="7"/>
+      <c r="C121" s="9"/>
     </row>
     <row r="122" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="str">
@@ -4901,7 +4901,7 @@
         <v/>
       </c>
       <c r="B122" s="7"/>
-      <c r="C122" s="7"/>
+      <c r="C122" s="9"/>
     </row>
     <row r="123" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="str">
@@ -4909,7 +4909,7 @@
         <v/>
       </c>
       <c r="B123" s="7"/>
-      <c r="C123" s="7"/>
+      <c r="C123" s="9"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="str">
@@ -4917,7 +4917,7 @@
         <v/>
       </c>
       <c r="B124" s="7"/>
-      <c r="C124" s="7"/>
+      <c r="C124" s="9"/>
     </row>
     <row r="125" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="str">
@@ -4925,7 +4925,7 @@
         <v/>
       </c>
       <c r="B125" s="7"/>
-      <c r="C125" s="7"/>
+      <c r="C125" s="9"/>
     </row>
     <row r="126" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="str">
@@ -4933,7 +4933,7 @@
         <v/>
       </c>
       <c r="B126" s="7"/>
-      <c r="C126" s="7"/>
+      <c r="C126" s="9"/>
     </row>
     <row r="127" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="str">
@@ -4941,7 +4941,7 @@
         <v/>
       </c>
       <c r="B127" s="7"/>
-      <c r="C127" s="7"/>
+      <c r="C127" s="9"/>
     </row>
     <row r="128" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="str">
@@ -4949,7 +4949,7 @@
         <v/>
       </c>
       <c r="B128" s="7"/>
-      <c r="C128" s="7"/>
+      <c r="C128" s="9"/>
     </row>
     <row r="129" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="str">
@@ -4957,7 +4957,7 @@
         <v/>
       </c>
       <c r="B129" s="7"/>
-      <c r="C129" s="7"/>
+      <c r="C129" s="9"/>
     </row>
     <row r="130" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="str">
@@ -4965,7 +4965,7 @@
         <v/>
       </c>
       <c r="B130" s="7"/>
-      <c r="C130" s="7"/>
+      <c r="C130" s="9"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="str">
@@ -4973,7 +4973,7 @@
         <v/>
       </c>
       <c r="B131" s="7"/>
-      <c r="C131" s="7"/>
+      <c r="C131" s="9"/>
     </row>
     <row r="132" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="str">
@@ -4981,7 +4981,7 @@
         <v/>
       </c>
       <c r="B132" s="7"/>
-      <c r="C132" s="7"/>
+      <c r="C132" s="9"/>
     </row>
     <row r="133" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="str">
@@ -4989,7 +4989,7 @@
         <v/>
       </c>
       <c r="B133" s="7"/>
-      <c r="C133" s="7"/>
+      <c r="C133" s="9"/>
     </row>
     <row r="134" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="str">
@@ -4997,7 +4997,7 @@
         <v/>
       </c>
       <c r="B134" s="7"/>
-      <c r="C134" s="7"/>
+      <c r="C134" s="9"/>
     </row>
     <row r="135" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="str">
@@ -5005,7 +5005,7 @@
         <v/>
       </c>
       <c r="B135" s="7"/>
-      <c r="C135" s="7"/>
+      <c r="C135" s="9"/>
     </row>
     <row r="136" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="str">
@@ -5013,7 +5013,7 @@
         <v/>
       </c>
       <c r="B136" s="7"/>
-      <c r="C136" s="7"/>
+      <c r="C136" s="9"/>
     </row>
     <row r="137" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="str">
@@ -5021,7 +5021,7 @@
         <v/>
       </c>
       <c r="B137" s="7"/>
-      <c r="C137" s="7"/>
+      <c r="C137" s="9"/>
     </row>
     <row r="138" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="str">
@@ -5029,7 +5029,7 @@
         <v/>
       </c>
       <c r="B138" s="7"/>
-      <c r="C138" s="7"/>
+      <c r="C138" s="9"/>
     </row>
     <row r="139" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="str">
@@ -5037,7 +5037,7 @@
         <v/>
       </c>
       <c r="B139" s="7"/>
-      <c r="C139" s="7"/>
+      <c r="C139" s="9"/>
     </row>
     <row r="140" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="str">
@@ -5045,7 +5045,7 @@
         <v/>
       </c>
       <c r="B140" s="7"/>
-      <c r="C140" s="7"/>
+      <c r="C140" s="9"/>
     </row>
     <row r="141" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="str">
@@ -5053,7 +5053,7 @@
         <v/>
       </c>
       <c r="B141" s="7"/>
-      <c r="C141" s="7"/>
+      <c r="C141" s="9"/>
     </row>
     <row r="142" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="str">
@@ -5061,7 +5061,7 @@
         <v/>
       </c>
       <c r="B142" s="7"/>
-      <c r="C142" s="7"/>
+      <c r="C142" s="9"/>
     </row>
     <row r="143" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="str">
@@ -5069,7 +5069,7 @@
         <v/>
       </c>
       <c r="B143" s="7"/>
-      <c r="C143" s="7"/>
+      <c r="C143" s="9"/>
     </row>
     <row r="144" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="str">
@@ -5077,7 +5077,7 @@
         <v/>
       </c>
       <c r="B144" s="7"/>
-      <c r="C144" s="7"/>
+      <c r="C144" s="9"/>
     </row>
     <row r="145" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="str">
@@ -5085,7 +5085,7 @@
         <v/>
       </c>
       <c r="B145" s="7"/>
-      <c r="C145" s="7"/>
+      <c r="C145" s="9"/>
     </row>
     <row r="146" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="str">
@@ -5093,7 +5093,7 @@
         <v/>
       </c>
       <c r="B146" s="7"/>
-      <c r="C146" s="7"/>
+      <c r="C146" s="9"/>
     </row>
     <row r="147" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="str">
@@ -5101,7 +5101,7 @@
         <v/>
       </c>
       <c r="B147" s="7"/>
-      <c r="C147" s="7"/>
+      <c r="C147" s="9"/>
     </row>
     <row r="148" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="str">
@@ -5109,7 +5109,7 @@
         <v/>
       </c>
       <c r="B148" s="7"/>
-      <c r="C148" s="7"/>
+      <c r="C148" s="9"/>
     </row>
     <row r="149" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="str">
@@ -5117,7 +5117,7 @@
         <v/>
       </c>
       <c r="B149" s="7"/>
-      <c r="C149" s="7"/>
+      <c r="C149" s="9"/>
     </row>
     <row r="150" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="str">
@@ -5125,7 +5125,7 @@
         <v/>
       </c>
       <c r="B150" s="7"/>
-      <c r="C150" s="7"/>
+      <c r="C150" s="9"/>
     </row>
     <row r="151" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="str">
@@ -5133,7 +5133,7 @@
         <v/>
       </c>
       <c r="B151" s="7"/>
-      <c r="C151" s="7"/>
+      <c r="C151" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>